<commit_message>
add 4 linked publication for CCHF, 1 for  Nipah virus, they're not found in pubmed search, and found by AI search
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/ReferenceSummary_Feb25.xlsx
+++ b/Pubmed/CCHF/ReferenceSummary_Feb25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindazhou/Desktop/HIV/GenBankRefs/Pubmed/CCHF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A455F3B-D83E-D540-8750-AB1EF63B4C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78D5F5D-1B99-9F4A-90B5-68F7AA3724AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1220" windowWidth="34260" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="500" windowWidth="34260" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3395" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3396" uniqueCount="948">
   <si>
     <t>Title</t>
   </si>
@@ -3591,6 +3591,9 @@
   <si>
     <t>Iran, Turkey</t>
   </si>
+  <si>
+    <t>JF922673, JF922674, JF922675, JF922676, JF922677, JF922678, JF922679</t>
+  </si>
 </sst>
 </file>
 
@@ -4126,9 +4129,9 @@
   </sheetPr>
   <dimension ref="A1:AW182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R58" sqref="R58"/>
+      <selection pane="bottomLeft" activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8472,7 +8475,9 @@
       <c r="R60" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="S60" s="2"/>
+      <c r="S60" s="2" t="s">
+        <v>947</v>
+      </c>
       <c r="T60" s="2" t="s">
         <v>357</v>
       </c>

</xml_diff>